<commit_message>
add collect data readme
</commit_message>
<xml_diff>
--- a/Aruco/Analyze/AnalyzeResult/summary.xlsx
+++ b/Aruco/Analyze/AnalyzeResult/summary.xlsx
@@ -32,7 +32,7 @@
     <t>Avg_Time_nHap</t>
   </si>
   <si>
-    <t>test</t>
+    <t>KuanWen</t>
   </si>
   <si>
     <t>Nan</t>
@@ -413,17 +413,17 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2" t="n">
+        <v>0.06561811251427289</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1937707000308567</v>
+        <v>5.122529692120022</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="n">
-        <v>0.219342311223348</v>
+        <v>0.1963057782914903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>